<commit_message>
adds excel preview generation to frontend
</commit_message>
<xml_diff>
--- a/apps/web-app/simple_test.xlsx
+++ b/apps/web-app/simple_test.xlsx
@@ -6,20 +6,121 @@
   <sheets>
     <sheet sheetId="1" name="Simple Property Survey" state="visible" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Simple Property Survey'!$B2:$H20</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Size (SF)</t>
-  </si>
-  <si>
-    <t>Asking Rate</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Address</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Size (SF)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Divisibility (SF)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>NNN Asking Rate (SF/Mo)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Opex (SF/Mo)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Direct/Sublease</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Comments</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>1</t>
+    </r>
   </si>
   <si>
     <t>401 Lambert Avenue, Palo Alto, CA 94306</t>
@@ -28,25 +129,79 @@
     <t>8000</t>
   </si>
   <si>
+    <t>3500 - 3500</t>
+  </si>
+  <si>
     <t>$4.00</t>
   </si>
   <si>
+    <t>Direct Lease</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Available within 60 days
+ - Open Floor Plan w/ 1 conference room (can build more)
+ - Kitchenette
+ - Two restrooms and a Shower
+ - 12 Parking Spaces in secure private garage Private outdoor balconies
+ - Call for pricing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
     <t>4101 El Camino Way, Palo Alto, CA 94306</t>
   </si>
   <si>
     <t>8975</t>
   </si>
   <si>
+    <t>2768 - 2768</t>
+  </si>
+  <si>
     <t>$4.50</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Rare stand-along retail building on El Camino Real
+ - 11 On-site parking spaces
+ - Restaurant infrastructure in place (fume hood, multiple walk-in refrigeration units)
+ - Tenant Improvements are available</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="0"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
     <t>366 Cambridge Ave, Palo Alto, CA 94306</t>
   </si>
   <si>
     <t>4029</t>
   </si>
   <si>
-    <t/>
+    <t>702 - 2717</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - After Hours HVAC Available, Air Conditioning, Balcony, Bicycle Storage, CCTV (Closed Circuit
+ - Television Monitoring), Central Heating, Conference Rooms, Hardwood Floors, Kitchen, Natural Light,
+ - Plug &amp; Play, Private Restrooms, Security System, Wi-Fi</t>
   </si>
 </sst>
 </file>
@@ -65,12 +220,17 @@
       <b/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF046BB6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,9 +245,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,58 +599,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:H4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="3" width="20" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="30" customHeight="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>